<commit_message>
new commit with update
</commit_message>
<xml_diff>
--- a/RAiSD/RAiSD_genes/raisd_gene_function.xlsx
+++ b/RAiSD/RAiSD_genes/raisd_gene_function.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wengz\Dropbox\Chapter 3\Nebria_ingens_WGS\RAiSD\RAiSD_genes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A2666C-1431-46A3-9842-37586D65F170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4971A0-6E45-4D4B-BCF7-9C04276072CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="top_genes" sheetId="2" r:id="rId1"/>
+    <sheet name="Pop_info" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="244">
   <si>
     <t>Nriv.00g061930</t>
   </si>
@@ -728,6 +729,78 @@
   </si>
   <si>
     <t>Keleg et al, 2014</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Army</t>
+  </si>
+  <si>
+    <t>Conness</t>
+  </si>
+  <si>
+    <t>Crabtree</t>
+  </si>
+  <si>
+    <t>Donohue</t>
+  </si>
+  <si>
+    <t>HungryPacker</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Lamarck</t>
+  </si>
+  <si>
+    <t>Lyell</t>
+  </si>
+  <si>
+    <t>Millys</t>
+  </si>
+  <si>
+    <t>Monarch</t>
+  </si>
+  <si>
+    <t>Pear</t>
+  </si>
+  <si>
+    <t>Piute</t>
+  </si>
+  <si>
+    <t>Recess</t>
+  </si>
+  <si>
+    <t>Ritter</t>
+  </si>
+  <si>
+    <t>Ruby</t>
+  </si>
+  <si>
+    <t>SamMack</t>
+  </si>
+  <si>
+    <t>Selden</t>
+  </si>
+  <si>
+    <t>SForester</t>
+  </si>
+  <si>
+    <t>Taboose</t>
+  </si>
+  <si>
+    <t>Treasure</t>
+  </si>
+  <si>
+    <t>Wright</t>
+  </si>
+  <si>
+    <t>Outlier_gene_count</t>
+  </si>
+  <si>
+    <t>Outlier_SNP_count</t>
   </si>
 </sst>
 </file>
@@ -1123,7 +1196,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:G1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2085,4 +2158,269 @@
   <pageSetup orientation="portrait" r:id="rId16"/>
   <legacyDrawing r:id="rId17"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CCDEA5A-49F0-4A99-BDC0-B367B34B7297}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A2:A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.90625" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="18.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B2">
+        <v>1415</v>
+      </c>
+      <c r="C2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3">
+        <v>2134</v>
+      </c>
+      <c r="C3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B4">
+        <v>2148</v>
+      </c>
+      <c r="C4">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5">
+        <v>2079</v>
+      </c>
+      <c r="C5">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B6">
+        <v>2558</v>
+      </c>
+      <c r="C6">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B7">
+        <v>2318</v>
+      </c>
+      <c r="C7">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B8">
+        <v>2142</v>
+      </c>
+      <c r="C8">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>240</v>
+      </c>
+      <c r="B9">
+        <v>2679</v>
+      </c>
+      <c r="C9">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B10">
+        <v>2520</v>
+      </c>
+      <c r="C10">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>237</v>
+      </c>
+      <c r="B11">
+        <v>2263</v>
+      </c>
+      <c r="C11">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>241</v>
+      </c>
+      <c r="B12">
+        <v>2377</v>
+      </c>
+      <c r="C12">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13">
+        <v>3074</v>
+      </c>
+      <c r="C13">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>226</v>
+      </c>
+      <c r="B14">
+        <v>2562</v>
+      </c>
+      <c r="C14">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B15">
+        <v>2875</v>
+      </c>
+      <c r="C15">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16">
+        <v>3140</v>
+      </c>
+      <c r="C16">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>224</v>
+      </c>
+      <c r="B17">
+        <v>3201</v>
+      </c>
+      <c r="C17">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>229</v>
+      </c>
+      <c r="B18">
+        <v>3019</v>
+      </c>
+      <c r="C18">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>225</v>
+      </c>
+      <c r="B19">
+        <v>2894</v>
+      </c>
+      <c r="C19">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>230</v>
+      </c>
+      <c r="B20">
+        <v>2423</v>
+      </c>
+      <c r="C20">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>233</v>
+      </c>
+      <c r="B21">
+        <v>2684</v>
+      </c>
+      <c r="C21">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>234</v>
+      </c>
+      <c r="B22">
+        <v>3200</v>
+      </c>
+      <c r="C22">
+        <v>479</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C24">
+    <sortCondition ref="C2:C24"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>